<commit_message>
uproszczenie uzycia DSP, mnozenie ze znakiem liczb z zakresu -2/2
</commit_message>
<xml_diff>
--- a/FPGA/States_table.xlsx
+++ b/FPGA/States_table.xlsx
@@ -101,6 +101,9 @@
     <t>M1H</t>
   </si>
   <si>
+    <t>M0H</t>
+  </si>
+  <si>
     <t>MULTA</t>
   </si>
   <si>
@@ -203,9 +206,6 @@
     <t>M0HS</t>
   </si>
   <si>
-    <t>M1HS</t>
-  </si>
-  <si>
     <t>Resonant state machine</t>
   </si>
   <si>
@@ -272,18 +272,6 @@
     <t>SM0_X2</t>
   </si>
   <si>
-    <t>SINC</t>
-  </si>
-  <si>
-    <t>CINC</t>
-  </si>
-  <si>
-    <t>SRST</t>
-  </si>
-  <si>
-    <t>CRST</t>
-  </si>
-  <si>
     <t>M0R ptr</t>
   </si>
   <si>
@@ -303,6 +291,18 @@
   </si>
   <si>
     <t>CM1_INP</t>
+  </si>
+  <si>
+    <t>S_INC</t>
+  </si>
+  <si>
+    <t>C_INC</t>
+  </si>
+  <si>
+    <t>S_RST</t>
+  </si>
+  <si>
+    <t>C_RST</t>
   </si>
 </sst>
 </file>
@@ -1410,7 +1410,7 @@
   <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1434,7 +1434,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="35" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1" s="36" t="s">
         <v>0</v>
@@ -1463,16 +1463,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="41" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E2" s="42" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F2" s="43" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G2" s="41" t="s">
         <v>2</v>
@@ -1505,10 +1505,10 @@
         <v>11</v>
       </c>
       <c r="Q2" s="40" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R2" s="43" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="S2" s="38"/>
     </row>
@@ -1518,13 +1518,13 @@
         <v>0</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="D3" s="48" t="s">
         <v>76</v>
       </c>
       <c r="E3" s="49" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="F3" s="50"/>
       <c r="G3" s="51"/>
@@ -1544,13 +1544,13 @@
       </c>
       <c r="P3" s="55"/>
       <c r="Q3" s="56" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="R3" s="55" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="S3" s="38" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
@@ -1570,22 +1570,22 @@
         <v>19</v>
       </c>
       <c r="H4" s="59" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="I4" s="59" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="J4" s="59" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="K4" s="63" t="s">
         <v>71</v>
       </c>
       <c r="L4" s="64" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M4" s="59" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N4" s="59" t="s">
         <v>71</v>
@@ -1616,28 +1616,28 @@
         <v>73</v>
       </c>
       <c r="G5" s="62" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="H5" s="60" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I5" s="60" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="J5" s="60" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K5" s="63" t="s">
         <v>71</v>
       </c>
       <c r="L5" s="58" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M5" s="60" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N5" s="60" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O5" s="66" t="s">
         <v>16</v>
@@ -1666,25 +1666,25 @@
         <v>19</v>
       </c>
       <c r="H6" s="59" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="I6" s="60" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="J6" s="60" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="K6" s="63" t="s">
         <v>71</v>
       </c>
       <c r="L6" s="58" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M6" s="60" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N6" s="60" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O6" s="66" t="s">
         <v>16</v>
@@ -1713,22 +1713,22 @@
         <v>19</v>
       </c>
       <c r="H7" s="60" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="I7" s="60" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="J7" s="60" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="K7" s="63" t="s">
         <v>71</v>
       </c>
       <c r="L7" s="58" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M7" s="60" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N7" s="60"/>
       <c r="O7" s="66" t="s">
@@ -1757,31 +1757,31 @@
         <v>73</v>
       </c>
       <c r="G8" s="62" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="H8" s="60" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I8" s="60" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="J8" s="60" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K8" s="63" t="s">
         <v>71</v>
       </c>
       <c r="L8" s="58" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M8" s="60" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N8" s="60" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O8" s="66" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="P8" s="67"/>
       <c r="Q8" s="65"/>
@@ -1805,23 +1805,23 @@
         <v>19</v>
       </c>
       <c r="H9" s="59" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="I9" s="59" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="J9" s="59" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="K9" s="69"/>
       <c r="L9" s="58" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M9" s="60" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N9" s="60" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O9" s="66" t="s">
         <v>16</v>
@@ -1839,13 +1839,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="58" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="D10" s="60" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="60" t="s">
         <v>85</v>
-      </c>
-      <c r="E10" s="60" t="s">
-        <v>78</v>
       </c>
       <c r="F10" s="67"/>
       <c r="G10" s="66"/>
@@ -1856,7 +1856,7 @@
         <v>14</v>
       </c>
       <c r="L10" s="58" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M10" s="60"/>
       <c r="N10" s="60" t="s">
@@ -1867,10 +1867,10 @@
       </c>
       <c r="P10" s="67"/>
       <c r="Q10" s="65" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="R10" s="61" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="S10" s="38" t="s">
         <v>62</v>
@@ -1884,10 +1884,10 @@
       <c r="C11" s="53"/>
       <c r="D11" s="48"/>
       <c r="E11" s="48" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="F11" s="55" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G11" s="51" t="s">
         <v>71</v>
@@ -1898,17 +1898,17 @@
       <c r="I11" s="48"/>
       <c r="J11" s="48"/>
       <c r="K11" s="70" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L11" s="53" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M11" s="48"/>
       <c r="N11" s="48" t="s">
         <v>15</v>
       </c>
       <c r="O11" s="54" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P11" s="55"/>
       <c r="Q11" s="71"/>
@@ -1943,12 +1943,12 @@
         <v>15</v>
       </c>
       <c r="O12" s="54" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P12" s="55"/>
       <c r="Q12" s="71"/>
       <c r="R12" s="50" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="S12" s="38"/>
     </row>
@@ -2112,13 +2112,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="47" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D17" s="49" t="s">
         <v>71</v>
       </c>
       <c r="E17" s="49" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="F17" s="50" t="s">
         <v>71</v>
@@ -2154,7 +2154,7 @@
         <v>71</v>
       </c>
       <c r="Q17" s="56" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="R17" s="50" t="s">
         <v>71</v>
@@ -2168,7 +2168,7 @@
       </c>
       <c r="C18" s="64"/>
       <c r="D18" s="59" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E18" s="59"/>
       <c r="F18" s="61" t="s">
@@ -2178,22 +2178,22 @@
         <v>19</v>
       </c>
       <c r="H18" s="59" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="I18" s="59" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="J18" s="59" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="K18" s="63" t="s">
         <v>71</v>
       </c>
       <c r="L18" s="64" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M18" s="59" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N18" s="59" t="s">
         <v>71</v>
@@ -2230,19 +2230,19 @@
         <v>71</v>
       </c>
       <c r="I19" s="62" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="J19" s="59" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K19" s="63" t="s">
         <v>14</v>
       </c>
       <c r="L19" s="64" t="s">
+        <v>26</v>
+      </c>
+      <c r="M19" s="59" t="s">
         <v>25</v>
-      </c>
-      <c r="M19" s="59" t="s">
-        <v>24</v>
       </c>
       <c r="N19" s="59" t="s">
         <v>15</v>
@@ -2266,7 +2266,7 @@
       </c>
       <c r="C20" s="64"/>
       <c r="D20" s="59" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E20" s="59"/>
       <c r="F20" s="61" t="s">
@@ -2276,22 +2276,22 @@
         <v>19</v>
       </c>
       <c r="H20" s="59" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="I20" s="59" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="J20" s="59" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="K20" s="63" t="s">
         <v>71</v>
       </c>
       <c r="L20" s="64" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M20" s="59" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N20" s="59" t="s">
         <v>71</v>
@@ -2314,31 +2314,31 @@
         <v>18</v>
       </c>
       <c r="C21" s="58" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="D21" s="59" t="s">
         <v>77</v>
       </c>
       <c r="E21" s="60" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="F21" s="61"/>
       <c r="G21" s="62"/>
       <c r="H21" s="59"/>
       <c r="I21" s="59" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="J21" s="59" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K21" s="63" t="s">
         <v>14</v>
       </c>
       <c r="L21" s="64" t="s">
+        <v>26</v>
+      </c>
+      <c r="M21" s="59" t="s">
         <v>25</v>
-      </c>
-      <c r="M21" s="59" t="s">
-        <v>24</v>
       </c>
       <c r="N21" s="59" t="s">
         <v>15</v>
@@ -2350,7 +2350,7 @@
         <v>71</v>
       </c>
       <c r="Q21" s="65" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="R21" s="61" t="s">
         <v>77</v>
@@ -2365,11 +2365,11 @@
         <v>19</v>
       </c>
       <c r="C22" s="47" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D22" s="48"/>
       <c r="E22" s="49" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="F22" s="55"/>
       <c r="G22" s="54"/>
@@ -2385,13 +2385,13 @@
       <c r="O22" s="54"/>
       <c r="P22" s="55"/>
       <c r="Q22" s="56" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="R22" s="50" t="s">
         <v>71</v>
       </c>
       <c r="S22" s="38" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2400,11 +2400,11 @@
         <v>20</v>
       </c>
       <c r="C23" s="48" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="D23" s="49"/>
       <c r="E23" s="48" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="F23" s="50"/>
       <c r="G23" s="51"/>
@@ -2418,11 +2418,11 @@
       <c r="O23" s="54"/>
       <c r="P23" s="55"/>
       <c r="Q23" s="48" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="R23" s="55"/>
       <c r="S23" s="38" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
@@ -2943,7 +2943,7 @@
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="38"/>
       <c r="B35" s="96" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C35" s="38"/>
       <c r="D35" s="38"/>
@@ -2999,7 +2999,7 @@
   <dimension ref="A1:U39"/>
   <sheetViews>
     <sheetView zoomScale="101" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3055,16 +3055,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G2" s="32" t="s">
         <v>2</v>
@@ -3097,13 +3097,13 @@
         <v>11</v>
       </c>
       <c r="Q2" s="32" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R2" s="33" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="S2" s="33" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="T2" s="34" t="s">
         <v>70</v>
@@ -3117,7 +3117,7 @@
       <c r="C3" s="12"/>
       <c r="D3" s="5"/>
       <c r="E3" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>58</v>
@@ -3127,7 +3127,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="5"/>
@@ -3139,10 +3139,10 @@
       </c>
       <c r="P3" s="7"/>
       <c r="Q3" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S3" s="5">
         <v>1</v>
@@ -3157,7 +3157,7 @@
       <c r="C4" s="12"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>69</v>
@@ -3207,7 +3207,7 @@
       <c r="S5" s="6"/>
       <c r="T5" s="10"/>
       <c r="U5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3216,13 +3216,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>18</v>
@@ -3234,17 +3234,17 @@
         <v>20</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>20</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N6" s="8"/>
       <c r="O6" s="8" t="s">
@@ -3264,41 +3264,41 @@
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K7" s="3"/>
       <c r="L7" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O7" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="P7" s="9"/>
       <c r="Q7" s="1"/>
@@ -3312,16 +3312,16 @@
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>19</v>
@@ -3330,20 +3330,20 @@
         <v>20</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J8" s="8" t="s">
         <v>20</v>
       </c>
       <c r="K8" s="3"/>
       <c r="L8" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O8" s="8" t="s">
         <v>16</v>
@@ -3360,16 +3360,16 @@
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>30</v>
-      </c>
       <c r="F9" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>19</v>
@@ -3378,20 +3378,20 @@
         <v>20</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J9" s="8" t="s">
         <v>20</v>
       </c>
       <c r="K9" s="3"/>
       <c r="L9" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N9" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O9" s="8" t="s">
         <v>16</v>
@@ -3416,25 +3416,25 @@
       <c r="G10" s="11"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K10" s="9"/>
       <c r="L10" s="1"/>
       <c r="M10" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N10" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O10" s="8" t="s">
         <v>16</v>
       </c>
       <c r="P10" s="9"/>
       <c r="Q10" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="R10" s="8" t="s">
         <v>12</v>
@@ -3450,13 +3450,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>18</v>
@@ -3468,17 +3468,17 @@
         <v>20</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J11" s="8" t="s">
         <v>20</v>
       </c>
       <c r="K11" s="3"/>
       <c r="L11" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N11" s="8"/>
       <c r="O11" s="8" t="s">
@@ -3498,38 +3498,38 @@
         <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K12" s="3"/>
       <c r="L12" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N12" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O12" s="8" t="s">
         <v>16</v>
@@ -3546,16 +3546,16 @@
         <v>10</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>19</v>
@@ -3564,20 +3564,20 @@
         <v>20</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J13" s="8" t="s">
         <v>20</v>
       </c>
       <c r="K13" s="3"/>
       <c r="L13" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O13" s="8" t="s">
         <v>16</v>
@@ -3594,16 +3594,16 @@
         <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>30</v>
-      </c>
       <c r="F14" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>19</v>
@@ -3612,23 +3612,23 @@
         <v>20</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J14" s="8" t="s">
         <v>20</v>
       </c>
       <c r="K14" s="3"/>
       <c r="L14" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M14" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N14" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O14" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P14" s="9">
         <v>0</v>
@@ -3644,35 +3644,35 @@
         <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="11"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K15" s="9"/>
       <c r="L15" s="1"/>
       <c r="M15" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O15" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="P15" s="9"/>
       <c r="Q15" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="R15" s="2" t="s">
         <v>17</v>
@@ -3682,7 +3682,7 @@
       </c>
       <c r="T15" s="3"/>
       <c r="U15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -3691,11 +3691,11 @@
         <v>13</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="12"/>
@@ -3709,7 +3709,7 @@
       <c r="O16" s="5"/>
       <c r="P16" s="7"/>
       <c r="Q16" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="R16" s="5"/>
       <c r="S16" s="6"/>
@@ -3721,16 +3721,16 @@
         <v>14</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G17" s="11" t="s">
         <v>19</v>
@@ -3739,17 +3739,17 @@
         <v>20</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K17" s="3"/>
       <c r="L17" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>15</v>
@@ -3771,41 +3771,41 @@
         <v>15</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K18" s="3"/>
       <c r="L18" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="M18" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="N18" s="2" t="s">
         <v>15</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="P18" s="3"/>
       <c r="Q18" s="11"/>
@@ -3818,16 +3818,16 @@
         <v>16</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G19" s="11" t="s">
         <v>19</v>
@@ -3836,17 +3836,17 @@
         <v>20</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K19" s="3"/>
       <c r="L19" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>15</v>
@@ -3868,11 +3868,11 @@
         <v>17</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="12"/>
@@ -3890,7 +3890,7 @@
       </c>
       <c r="P20" s="10"/>
       <c r="Q20" s="12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R20" s="6" t="s">
         <v>13</v>
@@ -3900,7 +3900,7 @@
       </c>
       <c r="T20" s="10"/>
       <c r="U20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.3">
@@ -3910,7 +3910,7 @@
       <c r="C21" s="12"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F21" s="10"/>
       <c r="G21" s="12"/>
@@ -3928,7 +3928,7 @@
       <c r="S21" s="6"/>
       <c r="T21" s="10"/>
       <c r="U21" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
testy DSP w MCU
</commit_message>
<xml_diff>
--- a/FPGA/States_table.xlsx
+++ b/FPGA/States_table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12015"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12012" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Kalman" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="77">
   <si>
     <t>Kalman state machine</t>
   </si>
@@ -874,6 +874,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -884,9 +887,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1206,56 +1206,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O5" zoomScale="116" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="1" customWidth="1"/>
     <col min="7" max="10" width="8" style="1" customWidth="1"/>
-    <col min="11" max="11" width="6.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="5.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="7.85546875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="11" width="6.5546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.88671875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="9.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="5.6640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="7.88671875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10.6640625" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+    <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="60"/>
-      <c r="P1" s="60"/>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="60"/>
-    </row>
-    <row r="2" spans="1:19" ht="38.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="62"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="61"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="61"/>
+    </row>
+    <row r="2" spans="1:19" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="63"/>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="8">
         <v>0</v>
@@ -1349,7 +1349,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="19">
         <v>1</v>
@@ -1397,7 +1397,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="19">
         <v>2</v>
@@ -1443,7 +1443,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="30"/>
       <c r="B6" s="19">
         <v>3</v>
@@ -1489,7 +1489,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="30"/>
       <c r="B7" s="19">
         <v>4</v>
@@ -1535,7 +1535,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="30"/>
       <c r="B8" s="19">
         <v>5</v>
@@ -1579,7 +1579,7 @@
       <c r="Q8" s="27"/>
       <c r="R8" s="29"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="30"/>
       <c r="B9" s="19">
         <v>6</v>
@@ -1623,7 +1623,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="30"/>
       <c r="B10" s="19">
         <v>7</v>
@@ -1666,7 +1666,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="30"/>
       <c r="B11" s="8">
         <v>8</v>
@@ -1709,7 +1709,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="30"/>
       <c r="B12" s="8">
         <v>9</v>
@@ -1732,7 +1732,7 @@
       <c r="L12" s="15"/>
       <c r="M12" s="10"/>
       <c r="N12" s="10" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="O12" s="16" t="s">
         <v>23</v>
@@ -1743,7 +1743,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="8">
         <v>10</v>
@@ -1771,7 +1771,7 @@
       <c r="Q13" s="33"/>
       <c r="R13" s="17"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="8">
         <v>11</v>
@@ -1807,7 +1807,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="8">
         <v>12</v>
@@ -1839,7 +1839,7 @@
       <c r="Q15" s="33"/>
       <c r="R15" s="17"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="8">
         <v>13</v>
@@ -1893,7 +1893,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="8">
         <v>14</v>
@@ -1947,7 +1947,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="19">
         <v>15</v>
@@ -1995,7 +1995,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="19">
         <v>16</v>
@@ -2043,7 +2043,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="19">
         <v>17</v>
@@ -2091,7 +2091,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="19">
         <v>18</v>
@@ -2142,7 +2142,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="8">
         <v>19</v>
@@ -2177,7 +2177,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="8">
         <v>20</v>
@@ -2208,7 +2208,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="36">
         <v>21</v>
@@ -2234,7 +2234,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="36">
         <v>22</v>
@@ -2260,7 +2260,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
       <c r="B26" s="36">
         <v>23</v>
@@ -2286,7 +2286,7 @@
       <c r="Q26" s="42"/>
       <c r="R26" s="39"/>
     </row>
-    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="47"/>
       <c r="B27" s="36">
         <v>24</v>
@@ -2334,7 +2334,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="49"/>
       <c r="B28" s="36">
         <v>25</v>
@@ -2388,7 +2388,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
       <c r="B29" s="36">
         <v>26</v>
@@ -2442,7 +2442,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" s="36">
         <v>27</v>
@@ -2496,7 +2496,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
       <c r="B31" s="36">
         <v>28</v>
@@ -2550,7 +2550,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
       <c r="B32" s="36">
         <v>29</v>
@@ -2604,7 +2604,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
       <c r="B33" s="36">
         <v>30</v>
@@ -2658,7 +2658,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="7"/>
       <c r="B34" s="51">
         <v>31</v>
@@ -2712,30 +2712,30 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B35" s="58"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
         <v>59</v>
       </c>
@@ -2755,56 +2755,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S41"/>
   <sheetViews>
-    <sheetView topLeftCell="L2" zoomScale="89" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="89" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="1" customWidth="1"/>
     <col min="7" max="10" width="8" style="1" customWidth="1"/>
-    <col min="11" max="11" width="6.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="5.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="7.85546875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="11" width="6.5546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.88671875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="9.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="5.6640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="7.88671875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10.6640625" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+    <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="62" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="60"/>
-      <c r="P1" s="60"/>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="60"/>
-    </row>
-    <row r="2" spans="1:19" ht="38.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="62"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="61"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="61"/>
+    </row>
+    <row r="2" spans="1:19" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="63"/>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2857,7 +2857,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="8">
         <v>0</v>
@@ -2889,7 +2889,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="8">
         <v>1</v>
@@ -2921,7 +2921,7 @@
       <c r="Q4" s="33"/>
       <c r="R4" s="12"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="8">
         <v>2</v>
@@ -2943,7 +2943,7 @@
       <c r="Q5" s="33"/>
       <c r="R5" s="12"/>
     </row>
-    <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="30"/>
       <c r="B6" s="19">
         <v>3</v>
@@ -2989,7 +2989,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="30"/>
       <c r="B7" s="19">
         <v>4</v>
@@ -3033,7 +3033,7 @@
       <c r="Q7" s="27"/>
       <c r="R7" s="29"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="30"/>
       <c r="B8" s="19">
         <v>5</v>
@@ -3075,7 +3075,7 @@
       <c r="Q8" s="27"/>
       <c r="R8" s="29"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="30"/>
       <c r="B9" s="19">
         <v>6</v>
@@ -3119,7 +3119,7 @@
       <c r="Q9" s="27"/>
       <c r="R9" s="23"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="30"/>
       <c r="B10" s="19">
         <v>7</v>
@@ -3153,7 +3153,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="30"/>
       <c r="B11" s="19">
         <v>8</v>
@@ -3201,7 +3201,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="30"/>
       <c r="B12" s="19">
         <v>9</v>
@@ -3247,7 +3247,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="19">
         <v>10</v>
@@ -3291,7 +3291,7 @@
       <c r="Q13" s="27"/>
       <c r="R13" s="23"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="19">
         <v>11</v>
@@ -3335,7 +3335,7 @@
       <c r="Q14" s="27"/>
       <c r="R14" s="23"/>
     </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="19">
         <v>12</v>
@@ -3378,7 +3378,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="8">
         <v>13</v>
@@ -3435,7 +3435,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="19">
         <v>14</v>
@@ -3483,7 +3483,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="19">
         <v>15</v>
@@ -3527,7 +3527,7 @@
       <c r="Q18" s="34"/>
       <c r="R18" s="23"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="19">
         <v>16</v>
@@ -3578,7 +3578,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="8">
         <v>17</v>
@@ -3617,7 +3617,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="8">
         <v>18</v>
@@ -3630,7 +3630,7 @@
         <v>57</v>
       </c>
       <c r="F21" s="12"/>
-      <c r="G21" s="63"/>
+      <c r="G21" s="59"/>
       <c r="H21" s="11"/>
       <c r="I21" s="13"/>
       <c r="J21" s="11"/>
@@ -3650,7 +3650,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="36">
         <v>19</v>
@@ -3672,7 +3672,7 @@
       <c r="Q22" s="50"/>
       <c r="R22" s="43"/>
     </row>
-    <row r="23" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="36">
         <v>20</v>
@@ -3694,7 +3694,7 @@
       <c r="Q23" s="42"/>
       <c r="R23" s="43"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="36">
         <v>21</v>
@@ -3716,7 +3716,7 @@
       <c r="Q24" s="50"/>
       <c r="R24" s="43"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="36">
         <v>22</v>
@@ -3738,7 +3738,7 @@
       <c r="Q25" s="38"/>
       <c r="R25" s="39"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
       <c r="B26" s="36">
         <v>23</v>
@@ -3764,7 +3764,7 @@
       <c r="Q26" s="42"/>
       <c r="R26" s="39"/>
     </row>
-    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="47"/>
       <c r="B27" s="36">
         <v>24</v>
@@ -3812,7 +3812,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="49"/>
       <c r="B28" s="36">
         <v>25</v>
@@ -3866,7 +3866,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
       <c r="B29" s="36">
         <v>26</v>
@@ -3920,7 +3920,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" s="36">
         <v>27</v>
@@ -3974,7 +3974,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
       <c r="B31" s="36">
         <v>28</v>
@@ -4028,7 +4028,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
       <c r="B32" s="36">
         <v>29</v>
@@ -4082,7 +4082,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
       <c r="B33" s="36">
         <v>30</v>
@@ -4136,7 +4136,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="7"/>
       <c r="B34" s="51">
         <v>31</v>
@@ -4190,25 +4190,25 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B35" s="58"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B39" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B41" s="1" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
poprawka Kalmana, liczenie kwadratu
</commit_message>
<xml_diff>
--- a/FPGA/States_table.xlsx
+++ b/FPGA/States_table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12012" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12012"/>
   </bookViews>
   <sheets>
     <sheet name="Kalman" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="78">
   <si>
     <t>Kalman state machine</t>
   </si>
@@ -212,9 +212,6 @@
     <t>C_RST</t>
   </si>
   <si>
-    <t>f</t>
-  </si>
-  <si>
     <t>Cycles = s * (11*h + 10)</t>
   </si>
   <si>
@@ -236,9 +233,6 @@
     <t>harmonics_inc &lt;= 1'b1;if(!harmonic_end) cnt &lt;= 5'd1;</t>
   </si>
   <si>
-    <t>harmonics_inc &lt;= 1'b1; if(!harmonic_end) cnt &lt;= 5'd15;</t>
-  </si>
-  <si>
     <t>SM1_COB</t>
   </si>
   <si>
@@ -267,6 +261,15 @@
   </si>
   <si>
     <t>harmonics_rst &lt;= 1'b1; series_inc &lt;= 1'b1; if(!series_end) cnt &lt;= 5'd0;</t>
+  </si>
+  <si>
+    <t>SM0_A</t>
+  </si>
+  <si>
+    <t>harmonics_inc &lt;= 1'b1; if(!harmonic_end) cnt &lt;= 5'd12;</t>
+  </si>
+  <si>
+    <t>RM0L</t>
   </si>
 </sst>
 </file>
@@ -1206,8 +1209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T28" sqref="T28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1663,7 +1666,7 @@
         <v>51</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
@@ -1706,7 +1709,7 @@
         <v>41</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
@@ -1776,11 +1779,15 @@
       <c r="B14" s="8">
         <v>11</v>
       </c>
-      <c r="C14" s="15"/>
+      <c r="C14" s="9" t="s">
+        <v>56</v>
+      </c>
       <c r="D14" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="10"/>
+      <c r="E14" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="F14" s="12" t="s">
         <v>41</v>
       </c>
@@ -1796,155 +1803,161 @@
       <c r="J14" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="K14" s="14"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="33"/>
+      <c r="K14" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="M14" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="N14" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="O14" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="P14" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q14" s="18" t="s">
+        <v>56</v>
+      </c>
       <c r="R14" s="12" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
-      <c r="B15" s="8">
+      <c r="B15" s="19">
         <v>12</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="J15" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="K15" s="14"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="33"/>
-      <c r="R15" s="17"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="22"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="L15" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="M15" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="N15" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="O15" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="P15" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="34"/>
+      <c r="R15" s="23" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
-      <c r="B16" s="8">
+      <c r="B16" s="19">
         <v>13</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="J16" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="K16" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="L16" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="M16" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="N16" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="O16" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="P16" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q16" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="R16" s="12" t="s">
-        <v>41</v>
-      </c>
+      <c r="C16" s="20"/>
+      <c r="D16" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="22"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="J16" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="K16" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="L16" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="M16" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="N16" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="O16" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="P16" s="29"/>
+      <c r="Q16" s="34"/>
+      <c r="R16" s="23"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
-      <c r="B17" s="8">
+      <c r="B17" s="19">
         <v>14</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="J17" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="K17" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="L17" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="M17" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="N17" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="O17" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="P17" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q17" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="R17" s="12" t="s">
-        <v>41</v>
+      <c r="C17" s="20"/>
+      <c r="D17" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="22"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="K17" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="L17" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="M17" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="N17" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="O17" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="34"/>
+      <c r="R17" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
@@ -2118,7 +2131,7 @@
         <v>12</v>
       </c>
       <c r="L21" s="26" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="M21" s="21" t="s">
         <v>21</v>
@@ -2139,7 +2152,7 @@
         <v>47</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
@@ -2174,7 +2187,7 @@
         <v>41</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2214,67 +2227,55 @@
         <v>21</v>
       </c>
       <c r="C24" s="37"/>
-      <c r="D24" s="38"/>
+      <c r="D24" s="45"/>
       <c r="E24" s="38"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
-      <c r="K24" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="L24" s="37"/>
-      <c r="M24" s="38"/>
-      <c r="N24" s="38"/>
-      <c r="O24" s="40"/>
-      <c r="P24" s="39"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="41"/>
+      <c r="L24" s="48"/>
+      <c r="M24" s="45"/>
+      <c r="N24" s="45"/>
+      <c r="O24" s="44"/>
+      <c r="P24" s="43"/>
       <c r="Q24" s="42"/>
-      <c r="R24" s="43" t="s">
-        <v>41</v>
-      </c>
+      <c r="R24" s="43"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="36">
         <v>22</v>
       </c>
-      <c r="C25" s="37"/>
+      <c r="C25" s="48"/>
       <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
+      <c r="E25" s="45"/>
       <c r="F25" s="39"/>
       <c r="G25" s="40"/>
       <c r="H25" s="38"/>
       <c r="I25" s="38"/>
       <c r="J25" s="38"/>
-      <c r="K25" s="41" t="s">
-        <v>41</v>
-      </c>
+      <c r="K25" s="41"/>
       <c r="L25" s="37"/>
       <c r="M25" s="38"/>
       <c r="N25" s="38"/>
       <c r="O25" s="40"/>
       <c r="P25" s="39"/>
-      <c r="Q25" s="42"/>
-      <c r="R25" s="43" t="s">
-        <v>41</v>
-      </c>
+      <c r="Q25" s="50"/>
+      <c r="R25" s="43"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
       <c r="B26" s="36">
         <v>23</v>
       </c>
-      <c r="C26" s="37"/>
-      <c r="D26" s="38"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="45"/>
       <c r="E26" s="38"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="44" t="s">
-        <v>41</v>
-      </c>
-      <c r="H26" s="45" t="s">
-        <v>41</v>
-      </c>
+      <c r="F26" s="43"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="45"/>
       <c r="I26" s="38"/>
       <c r="J26" s="38"/>
       <c r="K26" s="46"/>
@@ -2283,7 +2284,7 @@
       <c r="N26" s="38"/>
       <c r="O26" s="40"/>
       <c r="P26" s="39"/>
-      <c r="Q26" s="42"/>
+      <c r="Q26" s="38"/>
       <c r="R26" s="39"/>
     </row>
     <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2737,7 +2738,7 @@
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -2755,7 +2756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="89" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="89" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
@@ -2781,7 +2782,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="62" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="60" t="s">
         <v>33</v>
@@ -2866,7 +2867,7 @@
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G3" s="13"/>
       <c r="H3" s="11"/>
@@ -2900,7 +2901,7 @@
         <v>55</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="11"/>
@@ -2954,7 +2955,7 @@
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G6" s="28" t="s">
         <v>15</v>
@@ -3000,7 +3001,7 @@
       </c>
       <c r="E7" s="22"/>
       <c r="F7" s="29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G7" s="24" t="s">
         <v>17</v>
@@ -3044,7 +3045,7 @@
       </c>
       <c r="E8" s="22"/>
       <c r="F8" s="23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G8" s="24" t="s">
         <v>15</v>
@@ -3086,7 +3087,7 @@
       </c>
       <c r="E9" s="22"/>
       <c r="F9" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G9" s="24" t="s">
         <v>15</v>
@@ -3164,7 +3165,7 @@
       </c>
       <c r="E11" s="22"/>
       <c r="F11" s="29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G11" s="24" t="s">
         <v>15</v>
@@ -3212,7 +3213,7 @@
       </c>
       <c r="E12" s="22"/>
       <c r="F12" s="29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G12" s="24" t="s">
         <v>17</v>
@@ -3258,7 +3259,7 @@
       </c>
       <c r="E13" s="22"/>
       <c r="F13" s="23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G13" s="24" t="s">
         <v>15</v>
@@ -3302,7 +3303,7 @@
       </c>
       <c r="E14" s="22"/>
       <c r="F14" s="23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G14" s="24" t="s">
         <v>15</v>
@@ -3375,7 +3376,7 @@
         <v>47</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
@@ -3432,7 +3433,7 @@
         <v>41</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
@@ -3446,7 +3447,7 @@
       </c>
       <c r="E17" s="22"/>
       <c r="F17" s="23" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G17" s="24" t="s">
         <v>15</v>
@@ -3494,7 +3495,7 @@
       </c>
       <c r="E18" s="21"/>
       <c r="F18" s="23" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G18" s="24" t="s">
         <v>17</v>
@@ -3542,7 +3543,7 @@
         <v>54</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G19" s="24" t="s">
         <v>15</v>
@@ -3611,10 +3612,10 @@
         <v>56</v>
       </c>
       <c r="R20" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
@@ -4200,7 +4201,7 @@
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.3">
@@ -4210,7 +4211,7 @@
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B41" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
prace nad kompensacja harmonicznych
</commit_message>
<xml_diff>
--- a/FPGA/States_table.xlsx
+++ b/FPGA/States_table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14640" windowHeight="11265"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14640" windowHeight="11268" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Kalman" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="106">
   <si>
     <t>Kalman state machine</t>
   </si>
@@ -303,24 +303,6 @@
     <t>CM1_RT</t>
   </si>
   <si>
-    <t>if(!harmonic_end) cnt &lt;= 6'd2;</t>
-  </si>
-  <si>
-    <t>if(!harmonic_end) cnt &lt;= 6'd5;</t>
-  </si>
-  <si>
-    <t>if(!harmonic_end) cnt &lt;= 6'd16;</t>
-  </si>
-  <si>
-    <t>if(!harmonic_end) cnt &lt;= 6'd20;</t>
-  </si>
-  <si>
-    <t>if(!harmonic_end) cnt &lt;= 6'd25;</t>
-  </si>
-  <si>
-    <t>if(!harmonic_end) cnt &lt;= 6'd36;</t>
-  </si>
-  <si>
     <t>CM1_ZR</t>
   </si>
   <si>
@@ -357,7 +339,22 @@
     <t>Cycles = s * (32*h + 10)</t>
   </si>
   <si>
-    <t>zerowanie przed zapisem</t>
+    <t>harmonics_inc &lt;= 1'b1; if(!harmonic_end) cnt &lt;= 6'd2;</t>
+  </si>
+  <si>
+    <t>harmonics_inc &lt;= 1'b1; if(!harmonic_end) cnt &lt;= 6'd5;</t>
+  </si>
+  <si>
+    <t>harmonics_inc &lt;= 1'b1; if(!harmonic_end) cnt &lt;= 6'd16;</t>
+  </si>
+  <si>
+    <t>harmonics_inc &lt;= 1'b1; if(!harmonic_end) cnt &lt;= 6'd20;</t>
+  </si>
+  <si>
+    <t>harmonics_inc &lt;= 1'b1; if(!harmonic_end) cnt &lt;= 6'd25;</t>
+  </si>
+  <si>
+    <t>harmonics_inc &lt;= 1'b1; if(!harmonic_end) cnt &lt;= 6'd36;</t>
   </si>
 </sst>
 </file>
@@ -365,7 +362,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode=";;"/>
+    <numFmt numFmtId="164" formatCode=";;"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -971,19 +968,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -996,6 +981,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1315,56 +1312,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="1" customWidth="1"/>
     <col min="7" max="10" width="8" style="1" customWidth="1"/>
-    <col min="11" max="11" width="6.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="5.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="7.85546875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="11" width="6.5546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.88671875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="9.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="5.6640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="7.88671875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10.6640625" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="62" t="s">
+    <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="61"/>
-      <c r="P1" s="61"/>
-      <c r="Q1" s="61"/>
-      <c r="R1" s="61"/>
-    </row>
-    <row r="2" spans="1:19" ht="38.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="63"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+    </row>
+    <row r="2" spans="1:19" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="68"/>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1417,7 +1414,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="8">
         <v>0</v>
@@ -1456,7 +1453,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="19">
         <v>1</v>
@@ -1502,7 +1499,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="19">
         <v>2</v>
@@ -1546,7 +1543,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="30"/>
       <c r="B6" s="19">
         <v>3</v>
@@ -1590,7 +1587,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="30"/>
       <c r="B7" s="19">
         <v>4</v>
@@ -1634,7 +1631,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="30"/>
       <c r="B8" s="19">
         <v>5</v>
@@ -1678,7 +1675,7 @@
       <c r="Q8" s="27"/>
       <c r="R8" s="29"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="30"/>
       <c r="B9" s="19">
         <v>6</v>
@@ -1720,7 +1717,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="30"/>
       <c r="B10" s="19">
         <v>7</v>
@@ -1761,7 +1758,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="30"/>
       <c r="B11" s="8">
         <v>8</v>
@@ -1804,7 +1801,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="30"/>
       <c r="B12" s="8">
         <v>9</v>
@@ -1838,7 +1835,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="8">
         <v>10</v>
@@ -1866,7 +1863,7 @@
       <c r="Q13" s="33"/>
       <c r="R13" s="17"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="8">
         <v>11</v>
@@ -1920,7 +1917,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="19">
         <v>12</v>
@@ -1964,7 +1961,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="19">
         <v>13</v>
@@ -2004,7 +2001,7 @@
       <c r="Q16" s="34"/>
       <c r="R16" s="23"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="19">
         <v>14</v>
@@ -2046,7 +2043,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="19">
         <v>15</v>
@@ -2092,7 +2089,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="19">
         <v>16</v>
@@ -2138,7 +2135,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="19">
         <v>17</v>
@@ -2184,7 +2181,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="19">
         <v>18</v>
@@ -2233,7 +2230,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="8">
         <v>19</v>
@@ -2268,7 +2265,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="8">
         <v>20</v>
@@ -2299,7 +2296,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="36">
         <v>21</v>
@@ -2321,7 +2318,7 @@
       <c r="Q24" s="42"/>
       <c r="R24" s="43"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="36">
         <v>22</v>
@@ -2343,7 +2340,7 @@
       <c r="Q25" s="50"/>
       <c r="R25" s="43"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
       <c r="B26" s="36">
         <v>23</v>
@@ -2365,7 +2362,7 @@
       <c r="Q26" s="38"/>
       <c r="R26" s="39"/>
     </row>
-    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="47"/>
       <c r="B27" s="36">
         <v>24</v>
@@ -2413,7 +2410,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="49"/>
       <c r="B28" s="36">
         <v>25</v>
@@ -2467,7 +2464,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
       <c r="B29" s="36">
         <v>26</v>
@@ -2521,7 +2518,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" s="36">
         <v>27</v>
@@ -2575,7 +2572,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
       <c r="B31" s="36">
         <v>28</v>
@@ -2629,7 +2626,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
       <c r="B32" s="36">
         <v>29</v>
@@ -2683,7 +2680,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
       <c r="B33" s="36">
         <v>30</v>
@@ -2737,7 +2734,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="7"/>
       <c r="B34" s="51">
         <v>31</v>
@@ -2791,30 +2788,30 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B35" s="58"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B39" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
         <v>57</v>
       </c>
@@ -2835,55 +2832,55 @@
   <dimension ref="A1:S41"/>
   <sheetViews>
     <sheetView zoomScale="89" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="1" customWidth="1"/>
     <col min="7" max="10" width="8" style="1" customWidth="1"/>
-    <col min="11" max="11" width="6.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="5.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="7.85546875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="11" width="6.5546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.88671875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="9.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="5.6640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="7.88671875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10.6640625" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="62" t="s">
+    <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="61"/>
-      <c r="P1" s="61"/>
-      <c r="Q1" s="61"/>
-      <c r="R1" s="61"/>
-    </row>
-    <row r="2" spans="1:19" ht="38.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="63"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+    </row>
+    <row r="2" spans="1:19" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="68"/>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2936,7 +2933,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="8">
         <v>0</v>
@@ -2966,7 +2963,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="8">
         <v>1</v>
@@ -2996,7 +2993,7 @@
       <c r="Q4" s="33"/>
       <c r="R4" s="12"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="8">
         <v>2</v>
@@ -3018,7 +3015,7 @@
       <c r="Q5" s="33"/>
       <c r="R5" s="12"/>
     </row>
-    <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="30"/>
       <c r="B6" s="19">
         <v>3</v>
@@ -3062,7 +3059,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="30"/>
       <c r="B7" s="19">
         <v>4</v>
@@ -3106,7 +3103,7 @@
       <c r="Q7" s="27"/>
       <c r="R7" s="29"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="30"/>
       <c r="B8" s="19">
         <v>5</v>
@@ -3146,7 +3143,7 @@
       <c r="Q8" s="27"/>
       <c r="R8" s="29"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="30"/>
       <c r="B9" s="19">
         <v>6</v>
@@ -3188,7 +3185,7 @@
       <c r="Q9" s="27"/>
       <c r="R9" s="23"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="30"/>
       <c r="B10" s="19">
         <v>7</v>
@@ -3220,7 +3217,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="30"/>
       <c r="B11" s="19">
         <v>8</v>
@@ -3266,7 +3263,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="30"/>
       <c r="B12" s="19">
         <v>9</v>
@@ -3310,7 +3307,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="19">
         <v>10</v>
@@ -3352,7 +3349,7 @@
       <c r="Q13" s="27"/>
       <c r="R13" s="23"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="19">
         <v>11</v>
@@ -3394,7 +3391,7 @@
       <c r="Q14" s="27"/>
       <c r="R14" s="23"/>
     </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="19">
         <v>12</v>
@@ -3435,7 +3432,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="8">
         <v>13</v>
@@ -3492,7 +3489,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="19">
         <v>14</v>
@@ -3540,7 +3537,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="19">
         <v>15</v>
@@ -3584,7 +3581,7 @@
       <c r="Q18" s="34"/>
       <c r="R18" s="23"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="19">
         <v>16</v>
@@ -3633,7 +3630,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="8">
         <v>17</v>
@@ -3670,7 +3667,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="8">
         <v>18</v>
@@ -3703,7 +3700,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="36">
         <v>19</v>
@@ -3725,7 +3722,7 @@
       <c r="Q22" s="50"/>
       <c r="R22" s="43"/>
     </row>
-    <row r="23" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="36">
         <v>20</v>
@@ -3747,7 +3744,7 @@
       <c r="Q23" s="42"/>
       <c r="R23" s="43"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="36">
         <v>21</v>
@@ -3769,7 +3766,7 @@
       <c r="Q24" s="50"/>
       <c r="R24" s="43"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="36">
         <v>22</v>
@@ -3791,7 +3788,7 @@
       <c r="Q25" s="38"/>
       <c r="R25" s="39"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
       <c r="B26" s="36">
         <v>23</v>
@@ -3817,7 +3814,7 @@
       <c r="Q26" s="42"/>
       <c r="R26" s="39"/>
     </row>
-    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="47"/>
       <c r="B27" s="36">
         <v>24</v>
@@ -3865,7 +3862,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="49"/>
       <c r="B28" s="36">
         <v>25</v>
@@ -3919,7 +3916,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
       <c r="B29" s="36">
         <v>26</v>
@@ -3973,7 +3970,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" s="36">
         <v>27</v>
@@ -4027,7 +4024,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
       <c r="B31" s="36">
         <v>28</v>
@@ -4081,7 +4078,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
       <c r="B32" s="36">
         <v>29</v>
@@ -4135,7 +4132,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
       <c r="B33" s="36">
         <v>30</v>
@@ -4189,7 +4186,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="7"/>
       <c r="B34" s="51">
         <v>31</v>
@@ -4243,25 +4240,25 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B35" s="58"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B39" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B41" s="1" t="s">
         <v>59</v>
       </c>
@@ -4278,59 +4275,59 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X73"/>
+  <dimension ref="A1:S73"/>
   <sheetViews>
-    <sheetView zoomScale="79" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="1" customWidth="1"/>
     <col min="7" max="10" width="8" style="1" customWidth="1"/>
-    <col min="11" max="11" width="6.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="5.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="7.85546875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="11" width="6.5546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.88671875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="9.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="5.6640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="7.88671875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10.6640625" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="62" t="s">
+    <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="61"/>
-      <c r="P1" s="61"/>
-      <c r="Q1" s="61"/>
-      <c r="R1" s="61"/>
-    </row>
-    <row r="2" spans="1:19" ht="38.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="63"/>
-      <c r="B2" s="64">
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+    </row>
+    <row r="2" spans="1:19" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="68"/>
+      <c r="B2" s="60">
         <v>-1</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -4382,9 +4379,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
-      <c r="B3" s="65">
+      <c r="B3" s="61">
         <f t="shared" ref="B3:B4" si="0">B2+1</f>
         <v>0</v>
       </c>
@@ -4394,7 +4391,7 @@
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="12" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G3" s="13" t="s">
         <v>40</v>
@@ -4429,9 +4426,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
-      <c r="B4" s="65">
+      <c r="B4" s="61">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4441,7 +4438,7 @@
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="12" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>40</v>
@@ -4474,10 +4471,10 @@
       <c r="Q4" s="33"/>
       <c r="R4" s="17"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
-      <c r="B5" s="65">
-        <f t="shared" ref="B4:B6" si="1">B4+1</f>
+      <c r="B5" s="61">
+        <f t="shared" ref="B5:B6" si="1">B4+1</f>
         <v>2</v>
       </c>
       <c r="C5" s="15"/>
@@ -4486,7 +4483,7 @@
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="12" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G5" s="13" t="s">
         <v>40</v>
@@ -4521,9 +4518,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="30"/>
-      <c r="B6" s="65">
+      <c r="B6" s="61">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -4533,7 +4530,7 @@
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="12" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G6" s="13" t="s">
         <v>40</v>
@@ -4565,12 +4562,15 @@
       </c>
       <c r="Q6" s="33"/>
       <c r="R6" s="17" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="30"/>
-      <c r="B7" s="66">
+      <c r="B7" s="62">
         <f>B6+1</f>
         <v>4</v>
       </c>
@@ -4596,21 +4596,18 @@
       <c r="P7" s="29"/>
       <c r="Q7" s="34"/>
       <c r="R7" s="29"/>
-      <c r="S7" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="30"/>
-      <c r="B8" s="66">
-        <f t="shared" ref="B8:B44" si="2">B7+1</f>
+      <c r="B8" s="62">
+        <f t="shared" ref="B8:B43" si="2">B7+1</f>
         <v>5</v>
       </c>
       <c r="C8" s="20" t="s">
         <v>53</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E8" s="28" t="s">
         <v>53</v>
@@ -4641,12 +4638,12 @@
         <v>78</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="30"/>
-      <c r="B9" s="65">
+      <c r="B9" s="61">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
@@ -4678,7 +4675,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="30"/>
       <c r="B10" s="19">
         <f t="shared" si="2"/>
@@ -4686,7 +4683,7 @@
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="22" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E10" s="22"/>
       <c r="F10" s="29" t="s">
@@ -4723,7 +4720,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="30"/>
       <c r="B11" s="19">
         <f t="shared" si="2"/>
@@ -4731,7 +4728,7 @@
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="22" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E11" s="22"/>
       <c r="F11" s="29" t="s">
@@ -4768,7 +4765,7 @@
       <c r="Q11" s="27"/>
       <c r="R11" s="29"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="30"/>
       <c r="B12" s="19">
         <f t="shared" si="2"/>
@@ -4776,7 +4773,7 @@
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="22" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E12" s="22"/>
       <c r="F12" s="23" t="s">
@@ -4809,7 +4806,7 @@
       <c r="Q12" s="27"/>
       <c r="R12" s="29"/>
     </row>
-    <row r="13" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="19">
         <f t="shared" si="2"/>
@@ -4821,7 +4818,7 @@
       </c>
       <c r="E13" s="22"/>
       <c r="F13" s="23" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="G13" s="24" t="s">
         <v>14</v>
@@ -4852,7 +4849,7 @@
       <c r="Q13" s="27"/>
       <c r="R13" s="23"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="19">
         <f t="shared" si="2"/>
@@ -4882,10 +4879,10 @@
       <c r="P14" s="29"/>
       <c r="Q14" s="27"/>
       <c r="R14" s="29" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="19">
         <f t="shared" si="2"/>
@@ -4893,7 +4890,7 @@
       </c>
       <c r="C15" s="20"/>
       <c r="D15" s="21" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E15" s="22"/>
       <c r="F15" s="29" t="s">
@@ -4932,7 +4929,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="19">
         <f t="shared" si="2"/>
@@ -4940,7 +4937,7 @@
       </c>
       <c r="C16" s="20"/>
       <c r="D16" s="21" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E16" s="22"/>
       <c r="F16" s="29" t="s">
@@ -4977,7 +4974,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="19">
         <f t="shared" si="2"/>
@@ -4985,7 +4982,7 @@
       </c>
       <c r="C17" s="20"/>
       <c r="D17" s="22" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E17" s="22"/>
       <c r="F17" s="23" t="s">
@@ -5020,7 +5017,7 @@
       <c r="Q17" s="27"/>
       <c r="R17" s="23"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="19">
         <f t="shared" si="2"/>
@@ -5032,7 +5029,7 @@
       </c>
       <c r="E18" s="22"/>
       <c r="F18" s="23" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G18" s="24" t="s">
         <v>14</v>
@@ -5062,11 +5059,8 @@
       </c>
       <c r="Q18" s="27"/>
       <c r="R18" s="23"/>
-      <c r="S18" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="19">
         <f t="shared" si="2"/>
@@ -5102,15 +5096,15 @@
         <v>53</v>
       </c>
       <c r="R19" s="23" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
-      <c r="B20" s="65">
+      <c r="B20" s="61">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
@@ -5142,7 +5136,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="19">
         <f t="shared" si="2"/>
@@ -5150,11 +5144,11 @@
       </c>
       <c r="C21" s="20"/>
       <c r="D21" s="22" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E21" s="22"/>
       <c r="F21" s="23" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="G21" s="24" t="s">
         <v>14</v>
@@ -5187,7 +5181,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="19">
         <f t="shared" si="2"/>
@@ -5195,11 +5189,11 @@
       </c>
       <c r="C22" s="26"/>
       <c r="D22" s="21" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E22" s="21"/>
       <c r="F22" s="23" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G22" s="24" t="s">
         <v>16</v>
@@ -5231,11 +5225,8 @@
       <c r="P22" s="23"/>
       <c r="Q22" s="34"/>
       <c r="R22" s="23"/>
-      <c r="S22" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="19">
         <f t="shared" si="2"/>
@@ -5245,13 +5236,13 @@
         <v>53</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E23" s="21" t="s">
         <v>53</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G23" s="24" t="s">
         <v>14</v>
@@ -5284,12 +5275,12 @@
         <v>78</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
-      <c r="B24" s="65">
+      <c r="B24" s="61">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
@@ -5321,7 +5312,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="19">
         <f t="shared" si="2"/>
@@ -5366,7 +5357,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
       <c r="B26" s="19">
         <f t="shared" si="2"/>
@@ -5374,7 +5365,7 @@
       </c>
       <c r="C26" s="20"/>
       <c r="D26" s="21" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E26" s="22"/>
       <c r="F26" s="29" t="s">
@@ -5409,7 +5400,7 @@
       <c r="Q26" s="34"/>
       <c r="R26" s="29"/>
     </row>
-    <row r="27" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="47"/>
       <c r="B27" s="19">
         <f t="shared" si="2"/>
@@ -5417,7 +5408,7 @@
       </c>
       <c r="C27" s="26"/>
       <c r="D27" s="21" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E27" s="21"/>
       <c r="F27" s="29" t="s">
@@ -5449,11 +5440,8 @@
       <c r="P27" s="23"/>
       <c r="Q27" s="34"/>
       <c r="R27" s="29"/>
-      <c r="S27" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="49"/>
       <c r="B28" s="19">
         <f t="shared" ref="B28" si="3">B27+1</f>
@@ -5463,7 +5451,7 @@
         <v>53</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E28" s="21" t="s">
         <v>53</v>
@@ -5492,15 +5480,12 @@
         <v>78</v>
       </c>
       <c r="S28" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="X28" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
-      <c r="B29" s="65">
+      <c r="B29" s="61">
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
@@ -5532,7 +5517,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:24" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" s="19">
         <f t="shared" si="2"/>
@@ -5577,7 +5562,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
       <c r="B31" s="19">
         <f t="shared" si="2"/>
@@ -5622,7 +5607,7 @@
       <c r="Q31" s="27"/>
       <c r="R31" s="29"/>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
       <c r="B32" s="19">
         <f t="shared" si="2"/>
@@ -5663,7 +5648,7 @@
       <c r="Q32" s="27"/>
       <c r="R32" s="29"/>
     </row>
-    <row r="33" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
       <c r="B33" s="19">
         <f t="shared" si="2"/>
@@ -5706,7 +5691,7 @@
       <c r="Q33" s="27"/>
       <c r="R33" s="23"/>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" s="7"/>
       <c r="B34" s="19">
         <f t="shared" si="2"/>
@@ -5739,7 +5724,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B35" s="19">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -5785,7 +5770,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B36" s="19">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -5829,7 +5814,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B37" s="19">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -5871,7 +5856,7 @@
       <c r="Q37" s="27"/>
       <c r="R37" s="23"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B38" s="19">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -5912,11 +5897,8 @@
       </c>
       <c r="Q38" s="27"/>
       <c r="R38" s="23"/>
-      <c r="S38" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B39" s="19">
         <f t="shared" si="2"/>
         <v>36</v>
@@ -5954,11 +5936,11 @@
         <v>79</v>
       </c>
       <c r="S39" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B40" s="65">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B40" s="61">
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
@@ -5990,7 +5972,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B41" s="19">
         <f t="shared" si="2"/>
         <v>38</v>
@@ -6038,7 +6020,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B42" s="19">
         <f t="shared" si="2"/>
         <v>39</v>
@@ -6081,11 +6063,8 @@
       <c r="P42" s="23"/>
       <c r="Q42" s="34"/>
       <c r="R42" s="23"/>
-      <c r="S42" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B43" s="19">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -6131,11 +6110,11 @@
       </c>
       <c r="R43" s="23"/>
       <c r="S43" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B44" s="65">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B44" s="61">
         <f t="shared" ref="B44:B48" si="4">B43+1</f>
         <v>41</v>
       </c>
@@ -6171,8 +6150,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B45" s="65">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B45" s="61">
         <f t="shared" si="4"/>
         <v>42</v>
       </c>
@@ -6201,8 +6180,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B46" s="67">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B46" s="63">
         <f t="shared" si="4"/>
         <v>43</v>
       </c>
@@ -6210,7 +6189,7 @@
       <c r="D46" s="45"/>
       <c r="E46" s="45"/>
       <c r="F46" s="43"/>
-      <c r="G46" s="68"/>
+      <c r="G46" s="64"/>
       <c r="H46" s="45"/>
       <c r="I46" s="44"/>
       <c r="J46" s="45"/>
@@ -6223,8 +6202,8 @@
       <c r="Q46" s="50"/>
       <c r="R46" s="43"/>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B47" s="67">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B47" s="63">
         <f t="shared" si="4"/>
         <v>44</v>
       </c>
@@ -6232,7 +6211,7 @@
       <c r="D47" s="45"/>
       <c r="E47" s="45"/>
       <c r="F47" s="43"/>
-      <c r="G47" s="68"/>
+      <c r="G47" s="64"/>
       <c r="H47" s="45"/>
       <c r="I47" s="44"/>
       <c r="J47" s="45"/>
@@ -6245,8 +6224,8 @@
       <c r="Q47" s="50"/>
       <c r="R47" s="43"/>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B48" s="67">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B48" s="63">
         <f t="shared" si="4"/>
         <v>45</v>
       </c>
@@ -6254,7 +6233,7 @@
       <c r="D48" s="45"/>
       <c r="E48" s="45"/>
       <c r="F48" s="43"/>
-      <c r="G48" s="68"/>
+      <c r="G48" s="64"/>
       <c r="H48" s="45"/>
       <c r="I48" s="44"/>
       <c r="J48" s="45"/>
@@ -6267,16 +6246,16 @@
       <c r="Q48" s="50"/>
       <c r="R48" s="43"/>
     </row>
-    <row r="49" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B49" s="67">
-        <f t="shared" ref="B7:B49" si="5">B48+1</f>
+    <row r="49" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B49" s="63">
+        <f t="shared" ref="B49" si="5">B48+1</f>
         <v>46</v>
       </c>
       <c r="C49" s="48"/>
       <c r="D49" s="45"/>
       <c r="E49" s="45"/>
       <c r="F49" s="43"/>
-      <c r="G49" s="68"/>
+      <c r="G49" s="64"/>
       <c r="H49" s="45"/>
       <c r="I49" s="44"/>
       <c r="J49" s="45"/>
@@ -6289,8 +6268,8 @@
       <c r="Q49" s="50"/>
       <c r="R49" s="43"/>
     </row>
-    <row r="50" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B50" s="67">
+    <row r="50" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B50" s="63">
         <f t="shared" ref="B50:B56" si="6">B49+1</f>
         <v>47</v>
       </c>
@@ -6298,7 +6277,7 @@
       <c r="D50" s="45"/>
       <c r="E50" s="45"/>
       <c r="F50" s="43"/>
-      <c r="G50" s="68"/>
+      <c r="G50" s="64"/>
       <c r="H50" s="45"/>
       <c r="I50" s="44"/>
       <c r="J50" s="45"/>
@@ -6311,8 +6290,8 @@
       <c r="Q50" s="50"/>
       <c r="R50" s="43"/>
     </row>
-    <row r="51" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B51" s="67">
+    <row r="51" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B51" s="63">
         <f t="shared" si="6"/>
         <v>48</v>
       </c>
@@ -6320,7 +6299,7 @@
       <c r="D51" s="45"/>
       <c r="E51" s="45"/>
       <c r="F51" s="43"/>
-      <c r="G51" s="68"/>
+      <c r="G51" s="64"/>
       <c r="H51" s="45"/>
       <c r="I51" s="44"/>
       <c r="J51" s="45"/>
@@ -6333,8 +6312,8 @@
       <c r="Q51" s="50"/>
       <c r="R51" s="43"/>
     </row>
-    <row r="52" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B52" s="67">
+    <row r="52" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B52" s="63">
         <f t="shared" si="6"/>
         <v>49</v>
       </c>
@@ -6342,7 +6321,7 @@
       <c r="D52" s="45"/>
       <c r="E52" s="45"/>
       <c r="F52" s="43"/>
-      <c r="G52" s="68"/>
+      <c r="G52" s="64"/>
       <c r="H52" s="45"/>
       <c r="I52" s="44"/>
       <c r="J52" s="45"/>
@@ -6355,8 +6334,8 @@
       <c r="Q52" s="50"/>
       <c r="R52" s="43"/>
     </row>
-    <row r="53" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B53" s="67">
+    <row r="53" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B53" s="63">
         <f t="shared" si="6"/>
         <v>50</v>
       </c>
@@ -6364,7 +6343,7 @@
       <c r="D53" s="45"/>
       <c r="E53" s="45"/>
       <c r="F53" s="43"/>
-      <c r="G53" s="68"/>
+      <c r="G53" s="64"/>
       <c r="H53" s="45"/>
       <c r="I53" s="44"/>
       <c r="J53" s="45"/>
@@ -6377,8 +6356,8 @@
       <c r="Q53" s="50"/>
       <c r="R53" s="43"/>
     </row>
-    <row r="54" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B54" s="67">
+    <row r="54" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B54" s="63">
         <f t="shared" si="6"/>
         <v>51</v>
       </c>
@@ -6386,7 +6365,7 @@
       <c r="D54" s="45"/>
       <c r="E54" s="45"/>
       <c r="F54" s="43"/>
-      <c r="G54" s="68"/>
+      <c r="G54" s="64"/>
       <c r="H54" s="45"/>
       <c r="I54" s="44"/>
       <c r="J54" s="45"/>
@@ -6399,8 +6378,8 @@
       <c r="Q54" s="50"/>
       <c r="R54" s="43"/>
     </row>
-    <row r="55" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B55" s="67">
+    <row r="55" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B55" s="63">
         <f t="shared" si="6"/>
         <v>52</v>
       </c>
@@ -6408,7 +6387,7 @@
       <c r="D55" s="45"/>
       <c r="E55" s="45"/>
       <c r="F55" s="43"/>
-      <c r="G55" s="68"/>
+      <c r="G55" s="64"/>
       <c r="H55" s="45"/>
       <c r="I55" s="44"/>
       <c r="J55" s="45"/>
@@ -6421,8 +6400,8 @@
       <c r="Q55" s="50"/>
       <c r="R55" s="43"/>
     </row>
-    <row r="56" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B56" s="67">
+    <row r="56" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B56" s="63">
         <f t="shared" si="6"/>
         <v>53</v>
       </c>
@@ -6430,7 +6409,7 @@
       <c r="D56" s="45"/>
       <c r="E56" s="45"/>
       <c r="F56" s="43"/>
-      <c r="G56" s="68"/>
+      <c r="G56" s="64"/>
       <c r="H56" s="45"/>
       <c r="I56" s="44"/>
       <c r="J56" s="45"/>
@@ -6443,8 +6422,8 @@
       <c r="Q56" s="50"/>
       <c r="R56" s="43"/>
     </row>
-    <row r="57" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B57" s="67">
+    <row r="57" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B57" s="63">
         <f t="shared" ref="B57:B64" si="7">B56+1</f>
         <v>54</v>
       </c>
@@ -6452,7 +6431,7 @@
       <c r="D57" s="45"/>
       <c r="E57" s="45"/>
       <c r="F57" s="43"/>
-      <c r="G57" s="68"/>
+      <c r="G57" s="64"/>
       <c r="H57" s="45"/>
       <c r="I57" s="44"/>
       <c r="J57" s="45"/>
@@ -6465,8 +6444,8 @@
       <c r="Q57" s="50"/>
       <c r="R57" s="43"/>
     </row>
-    <row r="58" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B58" s="67">
+    <row r="58" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B58" s="63">
         <f t="shared" si="7"/>
         <v>55</v>
       </c>
@@ -6474,7 +6453,7 @@
       <c r="D58" s="45"/>
       <c r="E58" s="45"/>
       <c r="F58" s="43"/>
-      <c r="G58" s="68"/>
+      <c r="G58" s="64"/>
       <c r="H58" s="45"/>
       <c r="I58" s="44"/>
       <c r="J58" s="45"/>
@@ -6487,8 +6466,8 @@
       <c r="Q58" s="50"/>
       <c r="R58" s="43"/>
     </row>
-    <row r="59" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B59" s="67">
+    <row r="59" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B59" s="63">
         <f t="shared" si="7"/>
         <v>56</v>
       </c>
@@ -6496,7 +6475,7 @@
       <c r="D59" s="45"/>
       <c r="E59" s="45"/>
       <c r="F59" s="43"/>
-      <c r="G59" s="68"/>
+      <c r="G59" s="64"/>
       <c r="H59" s="45"/>
       <c r="I59" s="44"/>
       <c r="J59" s="45"/>
@@ -6509,8 +6488,8 @@
       <c r="Q59" s="50"/>
       <c r="R59" s="43"/>
     </row>
-    <row r="60" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B60" s="67">
+    <row r="60" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B60" s="63">
         <f t="shared" si="7"/>
         <v>57</v>
       </c>
@@ -6518,7 +6497,7 @@
       <c r="D60" s="45"/>
       <c r="E60" s="45"/>
       <c r="F60" s="43"/>
-      <c r="G60" s="68"/>
+      <c r="G60" s="64"/>
       <c r="H60" s="45"/>
       <c r="I60" s="44"/>
       <c r="J60" s="45"/>
@@ -6531,8 +6510,8 @@
       <c r="Q60" s="50"/>
       <c r="R60" s="43"/>
     </row>
-    <row r="61" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B61" s="67">
+    <row r="61" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B61" s="63">
         <f t="shared" si="7"/>
         <v>58</v>
       </c>
@@ -6540,7 +6519,7 @@
       <c r="D61" s="45"/>
       <c r="E61" s="45"/>
       <c r="F61" s="43"/>
-      <c r="G61" s="68"/>
+      <c r="G61" s="64"/>
       <c r="H61" s="45"/>
       <c r="I61" s="44"/>
       <c r="J61" s="45"/>
@@ -6553,8 +6532,8 @@
       <c r="Q61" s="50"/>
       <c r="R61" s="43"/>
     </row>
-    <row r="62" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B62" s="67">
+    <row r="62" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B62" s="63">
         <f t="shared" si="7"/>
         <v>59</v>
       </c>
@@ -6562,7 +6541,7 @@
       <c r="D62" s="45"/>
       <c r="E62" s="45"/>
       <c r="F62" s="43"/>
-      <c r="G62" s="68"/>
+      <c r="G62" s="64"/>
       <c r="H62" s="45"/>
       <c r="I62" s="44"/>
       <c r="J62" s="45"/>
@@ -6575,8 +6554,8 @@
       <c r="Q62" s="50"/>
       <c r="R62" s="43"/>
     </row>
-    <row r="63" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B63" s="67">
+    <row r="63" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B63" s="63">
         <f t="shared" si="7"/>
         <v>60</v>
       </c>
@@ -6584,7 +6563,7 @@
       <c r="D63" s="45"/>
       <c r="E63" s="45"/>
       <c r="F63" s="43"/>
-      <c r="G63" s="68"/>
+      <c r="G63" s="64"/>
       <c r="H63" s="45"/>
       <c r="I63" s="44"/>
       <c r="J63" s="45"/>
@@ -6597,8 +6576,8 @@
       <c r="Q63" s="50"/>
       <c r="R63" s="43"/>
     </row>
-    <row r="64" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B64" s="67">
+    <row r="64" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B64" s="63">
         <f t="shared" si="7"/>
         <v>61</v>
       </c>
@@ -6606,7 +6585,7 @@
       <c r="D64" s="45"/>
       <c r="E64" s="45"/>
       <c r="F64" s="43"/>
-      <c r="G64" s="68"/>
+      <c r="G64" s="64"/>
       <c r="H64" s="45"/>
       <c r="I64" s="44"/>
       <c r="J64" s="45"/>
@@ -6619,8 +6598,8 @@
       <c r="Q64" s="50"/>
       <c r="R64" s="43"/>
     </row>
-    <row r="65" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B65" s="67">
+    <row r="65" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B65" s="63">
         <f t="shared" ref="B65:B66" si="8">B64+1</f>
         <v>62</v>
       </c>
@@ -6628,7 +6607,7 @@
       <c r="D65" s="45"/>
       <c r="E65" s="45"/>
       <c r="F65" s="43"/>
-      <c r="G65" s="68"/>
+      <c r="G65" s="64"/>
       <c r="H65" s="45"/>
       <c r="I65" s="44"/>
       <c r="J65" s="45"/>
@@ -6641,8 +6620,8 @@
       <c r="Q65" s="50"/>
       <c r="R65" s="43"/>
     </row>
-    <row r="66" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B66" s="67">
+    <row r="66" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B66" s="63">
         <f t="shared" si="8"/>
         <v>63</v>
       </c>
@@ -6650,7 +6629,7 @@
       <c r="D66" s="45"/>
       <c r="E66" s="45"/>
       <c r="F66" s="43"/>
-      <c r="G66" s="68"/>
+      <c r="G66" s="64"/>
       <c r="H66" s="45"/>
       <c r="I66" s="44"/>
       <c r="J66" s="45"/>
@@ -6663,24 +6642,24 @@
       <c r="Q66" s="50"/>
       <c r="R66" s="43"/>
     </row>
-    <row r="69" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B69" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="70" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B70" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B71" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="73" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B73" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dzialajaca kompensacja harmonicznych sieci
</commit_message>
<xml_diff>
--- a/FPGA/States_table.xlsx
+++ b/FPGA/States_table.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="106">
   <si>
     <t>Kalman state machine</t>
   </si>
@@ -339,22 +339,22 @@
     <t>Cycles = s * (32*h + 10)</t>
   </si>
   <si>
-    <t>harmonics_inc &lt;= 1'b1; if(!harmonic_end) cnt &lt;= 6'd2;</t>
-  </si>
-  <si>
-    <t>harmonics_inc &lt;= 1'b1; if(!harmonic_end) cnt &lt;= 6'd5;</t>
-  </si>
-  <si>
-    <t>harmonics_inc &lt;= 1'b1; if(!harmonic_end) cnt &lt;= 6'd16;</t>
-  </si>
-  <si>
-    <t>harmonics_inc &lt;= 1'b1; if(!harmonic_end) cnt &lt;= 6'd20;</t>
-  </si>
-  <si>
-    <t>harmonics_inc &lt;= 1'b1; if(!harmonic_end) cnt &lt;= 6'd25;</t>
-  </si>
-  <si>
-    <t>harmonics_inc &lt;= 1'b1; if(!harmonic_end) cnt &lt;= 6'd36;</t>
+    <t>harmonics_inc &lt;= 1'b1; if(!harmonic_end) cnt &lt;= 6'd4;</t>
+  </si>
+  <si>
+    <t>harmonics_inc &lt;= 1'b1; if(!harmonic_end) cnt &lt;= 6'd7;</t>
+  </si>
+  <si>
+    <t>harmonics_inc &lt;= 1'b1; if(!harmonic_end) cnt &lt;= 6'd18;</t>
+  </si>
+  <si>
+    <t>harmonics_inc &lt;= 1'b1; if(!harmonic_end) cnt &lt;= 6'd22;</t>
+  </si>
+  <si>
+    <t>harmonics_inc &lt;= 1'b1; if(!harmonic_end) cnt &lt;= 6'd27;</t>
+  </si>
+  <si>
+    <t>harmonics_inc &lt;= 1'b1; if(!harmonic_end) cnt &lt;= 6'd38;</t>
   </si>
 </sst>
 </file>
@@ -4278,7 +4278,7 @@
   <dimension ref="A1:S73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="N3" sqref="N3:N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4405,18 +4405,14 @@
       <c r="J3" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="K3" s="14" t="s">
-        <v>23</v>
-      </c>
+      <c r="K3" s="14"/>
       <c r="L3" s="15" t="s">
         <v>40</v>
       </c>
       <c r="M3" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="11" t="s">
-        <v>13</v>
-      </c>
+      <c r="N3" s="11"/>
       <c r="O3" s="13"/>
       <c r="P3" s="17" t="s">
         <v>40</v>
@@ -4452,18 +4448,14 @@
       <c r="J4" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="14" t="s">
-        <v>23</v>
-      </c>
+      <c r="K4" s="14"/>
       <c r="L4" s="15" t="s">
         <v>40</v>
       </c>
       <c r="M4" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="N4" s="11" t="s">
-        <v>13</v>
-      </c>
+      <c r="N4" s="11"/>
       <c r="O4" s="13"/>
       <c r="P4" s="17" t="s">
         <v>40</v>
@@ -4497,18 +4489,14 @@
       <c r="J5" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="K5" s="14" t="s">
-        <v>23</v>
-      </c>
+      <c r="K5" s="14"/>
       <c r="L5" s="15" t="s">
         <v>40</v>
       </c>
       <c r="M5" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="N5" s="11" t="s">
-        <v>13</v>
-      </c>
+      <c r="N5" s="11"/>
       <c r="O5" s="13"/>
       <c r="P5" s="17" t="s">
         <v>40</v>
@@ -5320,7 +5308,7 @@
       </c>
       <c r="C25" s="20"/>
       <c r="D25" s="21" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="E25" s="22"/>
       <c r="F25" s="29" t="s">
@@ -5365,7 +5353,7 @@
       </c>
       <c r="C26" s="20"/>
       <c r="D26" s="21" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="E26" s="22"/>
       <c r="F26" s="29" t="s">
@@ -5395,7 +5383,9 @@
       <c r="N26" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="O26" s="24"/>
+      <c r="O26" s="28" t="s">
+        <v>29</v>
+      </c>
       <c r="P26" s="29"/>
       <c r="Q26" s="34"/>
       <c r="R26" s="29"/>
@@ -5408,7 +5398,7 @@
       </c>
       <c r="C27" s="26"/>
       <c r="D27" s="21" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="E27" s="21"/>
       <c r="F27" s="29" t="s">

</xml_diff>